<commit_message>
Updated projects to fix hardcoded filepaths to be relative, and removed database password
</commit_message>
<xml_diff>
--- a/PersonInfoWebAPIWPF/PersonInfoWPFApp/Files/full_name.xlsx
+++ b/PersonInfoWebAPIWPF/PersonInfoWPFApp/Files/full_name.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>First Name</t>
   </si>
@@ -30,12 +30,34 @@
   <si>
     <t>asdf</t>
   </si>
+  <si>
+    <t>qwer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="21">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
@@ -102,7 +124,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1002"/>
+  <dimension ref="A1:B1013"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
@@ -4126,6 +4148,94 @@
       <c r="A1002" s="6"/>
       <c r="B1002" s="6"/>
     </row>
+    <row r="1003">
+      <c r="A1003" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1003" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1004" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1005" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1006" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1007" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1008" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1009" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1010" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1011" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1012" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1013" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>